<commit_message>
Update charset reference file
</commit_message>
<xml_diff>
--- a/charset.xlsx
+++ b/charset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\Desktop\poj_font_tutorial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\Documents\taigi\POJFonts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="302">
   <si>
     <t>A̍</t>
   </si>
@@ -921,6 +921,15 @@
   </si>
   <si>
     <t>uni x3</t>
+  </si>
+  <si>
+    <t>TONE TABLES</t>
+  </si>
+  <si>
+    <t>UNICODE LATIN</t>
+  </si>
+  <si>
+    <t>UNICODE LATIN (EXTENDED)</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1229,6 +1238,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1510,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A2:Q49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="48" x14ac:dyDescent="0.85"/>
@@ -1537,14 +1550,9 @@
     <col min="17" max="17" width="11.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.85">
-      <c r="B1" s="22"/>
-      <c r="C1" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="3" t="s">
-        <v>298</v>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.85">
+      <c r="B2" s="30" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.85">
@@ -1775,7 +1783,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.85">
       <c r="B9" s="2" t="s">
         <v>127</v>
       </c>
@@ -1811,12 +1819,6 @@
       </c>
       <c r="M9" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="P9" s="20" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.85">
@@ -1856,14 +1858,8 @@
       <c r="M10" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="O10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.85">
       <c r="B11" s="2" t="s">
         <v>151</v>
       </c>
@@ -1888,811 +1884,1291 @@
       <c r="I11" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="P11" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B13" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="M13" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="O13" s="20" t="s">
-        <v>280</v>
-      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.85">
+      <c r="B13" s="30" t="s">
+        <v>301</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="17"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.85">
       <c r="B14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="E14" s="29" t="s">
         <v>162</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="29" t="s">
         <v>164</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>1</v>
+        <v>165</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>168</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>1</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="17"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.85">
       <c r="B15" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="17"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.85">
+      <c r="B16" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="I16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="17"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B17" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="M17" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="17"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B18" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="M18" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="O18" s="4"/>
+      <c r="P18" s="17"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B19" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="I19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="17"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B20" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I20" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="K20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="17"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B21" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="17"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B22" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="K22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="17"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B23" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="G23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="17"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B24" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="K24" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="M24" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="O24" s="4"/>
+      <c r="P24" s="17"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B25" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>262</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="M25" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="O25" s="4"/>
+      <c r="P25" s="17"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B26" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="M26" s="29"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="C27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="M27" s="29"/>
+    </row>
+    <row r="28" spans="2:17" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B28" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="M28" s="29"/>
+    </row>
+    <row r="29" spans="2:17" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B29" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="N29" s="28"/>
+      <c r="O29" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="Q30"/>
+    </row>
+    <row r="31" spans="2:17" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B31" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="K31" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="L31" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="M31" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="O31" s="20" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.85">
+      <c r="B32" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.85">
+      <c r="B33" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I33" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J33" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K15" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" s="2" t="s">
+      <c r="K33" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="N33" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O15" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B16" s="2" t="s">
+      <c r="O33" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B34" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="J34" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="2" t="s">
+      <c r="K34" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M34" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="N16" s="7" t="s">
+      <c r="N34" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O16" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B17" s="2" t="s">
+      <c r="O34" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B35" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D35" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="15" t="s">
+      <c r="E35" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="15" t="s">
+      <c r="G35" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4" t="s">
+      <c r="I35" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" s="15" t="s">
+      <c r="K35" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="N17" s="4" t="s">
+      <c r="M35" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N35" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O17" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B18" s="2" t="s">
+      <c r="O35" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B36" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F36" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="13" t="s">
+      <c r="G36" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4" t="s">
+      <c r="I36" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="13" t="s">
+      <c r="K36" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="M18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="N18" s="13" t="s">
+      <c r="M36" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N36" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B19" s="2" t="s">
+      <c r="O36" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B37" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I37" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J37" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L19" s="2" t="s">
+      <c r="K37" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L37" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="M37" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="N37" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="O37" s="3" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="49.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A20" s="17"/>
-      <c r="B20" s="11" t="s">
+    <row r="38" spans="1:15" ht="49.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A38" s="17"/>
+      <c r="B38" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="24" t="s">
+      <c r="C38" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="24" t="s">
+      <c r="E38" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="24" t="s">
+      <c r="G38" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="J20" s="26" t="s">
+      <c r="I38" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="L20" s="24" t="s">
+      <c r="K38" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="L38" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="N20" s="24" t="s">
+      <c r="M38" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="N38" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="O20" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B21" s="2" t="s">
+      <c r="O38" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B39" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I39" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J39" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L21" s="2" t="s">
+      <c r="K39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="M39" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="N39" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="O21" s="3" t="s">
+      <c r="O39" s="3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A23" s="20"/>
-      <c r="B23" s="18" t="s">
+    <row r="41" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A41" s="20"/>
+      <c r="B41" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C41" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D41" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E41" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F41" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G41" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H41" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I41" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="K23" s="20" t="s">
+      <c r="K41" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="L23" s="18" t="s">
+      <c r="L41" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="M23" s="19" t="s">
+      <c r="M41" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="N41" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="O23" s="20" t="s">
+      <c r="O41" s="20" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.85">
-      <c r="B24" s="2" t="s">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.85">
+      <c r="B42" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I42" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J42" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L24" s="2" t="s">
+      <c r="K42" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L42" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="M42" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N42" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O24" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.85">
-      <c r="B25" s="2" t="s">
+      <c r="O42" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.85">
+      <c r="B43" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I43" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J43" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K25" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L25" s="2" t="s">
+      <c r="K43" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="M43" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="N25" s="7" t="s">
+      <c r="N43" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="O25" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B26" s="2" t="s">
+      <c r="O43" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B44" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I44" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J44" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L26" s="2" t="s">
+      <c r="K44" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L44" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="M44" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="N26" s="7" t="s">
+      <c r="N44" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="O26" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B27" s="2" t="s">
+      <c r="O44" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B45" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="15" t="s">
+      <c r="E45" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27" s="15" t="s">
+      <c r="G45" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H45" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I27" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J27" s="4" t="s">
+      <c r="I45" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J45" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L27" s="15" t="s">
+      <c r="K45" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L45" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="M27" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="N27" s="4" t="s">
+      <c r="M45" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N45" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="O27" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B28" s="2" t="s">
+      <c r="O45" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B46" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F46" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H28" s="13" t="s">
+      <c r="G46" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I28" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J28" s="4" t="s">
+      <c r="I46" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J46" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K28" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L28" s="13" t="s">
+      <c r="K46" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L46" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M28" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="N28" s="13" t="s">
+      <c r="M46" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N46" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="O28" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B29" s="2" t="s">
+      <c r="O46" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B47" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G47" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I47" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="J47" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K29" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L29" s="2" t="s">
+      <c r="K47" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="M47" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="N47" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="O29" s="3" t="s">
+      <c r="O47" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="49.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A30" s="21"/>
-      <c r="B30" s="11" t="s">
+    <row r="48" spans="1:15" ht="49.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A48" s="21"/>
+      <c r="B48" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="24" t="s">
+      <c r="C48" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="24" t="s">
+      <c r="E48" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="24" t="s">
+      <c r="G48" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H48" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="J30" s="26" t="s">
+      <c r="I48" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J48" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="K30" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="L30" s="24" t="s">
+      <c r="K48" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="L48" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="M30" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="N30" s="24" t="s">
+      <c r="M48" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="N48" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="O30" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B31" s="2" t="s">
+      <c r="O48" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B49" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I49" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="J49" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K31" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L31" s="2" t="s">
+      <c r="K49" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L49" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M49" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="N49" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="O31" s="3" t="s">
+      <c r="O49" s="3" t="s">
         <v>270</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add t6 characters for GochiHandPOJ
</commit_message>
<xml_diff>
--- a/charset.xlsx
+++ b/charset.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\Documents\taigi\POJFonts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miau/projects/POJFonts/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FB1A8D-A73D-5D42-B928-3408158A8841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31950" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31960" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="334">
   <si>
     <t>A̍</t>
   </si>
@@ -930,24 +931,151 @@
   </si>
   <si>
     <t>UNICODE LATIN (EXTENDED)</t>
+  </si>
+  <si>
+    <t> ˆ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>˘</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ˇ</t>
+  </si>
+  <si>
+    <t>U+030C</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ǎ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ě</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ǐ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>M̌</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ň</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ǒ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ǒ͘</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ǔ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+01D3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+01D1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+0147</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+01CF</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+011A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+01CD</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ǎ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ě</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ǐ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>m̌</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ň</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ǒ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ǒ͘</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ǔ</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+0148</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+01D2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+01D4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+01D0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+011B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>U+01CE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -959,6 +1087,18 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Nunito"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="32"/>
+      <color rgb="FF333333"/>
       <name val="Nunito"/>
     </font>
   </fonts>
@@ -1155,7 +1295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1243,9 +1383,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1522,40 +1675,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="48" x14ac:dyDescent="0.85"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="40"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="12" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.796875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="7.796875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.59765625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.19921875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.59765625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.796875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="11.59765625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="7.796875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.3984375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="2" spans="2:16">
       <c r="B2" s="30" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="3" spans="2:16">
       <c r="B3" s="2" t="s">
         <v>55</v>
       </c>
@@ -1593,7 +1746,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="4" spans="2:16">
       <c r="B4" s="2" t="s">
         <v>67</v>
       </c>
@@ -1631,7 +1784,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="5" spans="2:16">
       <c r="B5" s="2" t="s">
         <v>79</v>
       </c>
@@ -1669,7 +1822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="6" spans="2:16">
       <c r="B6" s="2" t="s">
         <v>91</v>
       </c>
@@ -1707,7 +1860,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="7" spans="2:16">
       <c r="B7" s="2" t="s">
         <v>103</v>
       </c>
@@ -1745,7 +1898,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="8" spans="2:16">
       <c r="B8" s="2" t="s">
         <v>115</v>
       </c>
@@ -1783,7 +1936,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="9" spans="2:16">
       <c r="B9" s="2" t="s">
         <v>127</v>
       </c>
@@ -1821,7 +1974,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="10" spans="2:16">
       <c r="B10" s="2" t="s">
         <v>139</v>
       </c>
@@ -1859,7 +2012,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
         <v>151</v>
       </c>
@@ -1885,14 +2038,14 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="13" spans="2:16">
       <c r="B13" s="30" t="s">
         <v>301</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="17"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="14" spans="2:16">
       <c r="B14" s="2" t="s">
         <v>159</v>
       </c>
@@ -1932,7 +2085,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="17"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="15" spans="2:16">
       <c r="B15" s="2" t="s">
         <v>171</v>
       </c>
@@ -1972,7 +2125,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="17"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.85">
+    <row r="16" spans="2:16">
       <c r="B16" s="2" t="s">
         <v>183</v>
       </c>
@@ -1997,7 +2150,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="17"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="17" spans="2:16">
       <c r="B17" s="2" t="s">
         <v>189</v>
       </c>
@@ -2037,7 +2190,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="17"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="18" spans="2:16">
       <c r="B18" s="2" t="s">
         <v>201</v>
       </c>
@@ -2077,7 +2230,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="17"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="19" spans="2:16">
       <c r="B19" s="2" t="s">
         <v>213</v>
       </c>
@@ -2102,7 +2255,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="17"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="20" spans="2:16">
       <c r="B20" s="2" t="s">
         <v>219</v>
       </c>
@@ -2132,7 +2285,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="17"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="21" spans="2:16">
       <c r="B21" s="2" t="s">
         <v>227</v>
       </c>
@@ -2157,12 +2310,22 @@
       <c r="I21" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="K21" s="29"/>
-      <c r="M21" s="29"/>
+      <c r="J21" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="M21" s="29" t="s">
+        <v>332</v>
+      </c>
       <c r="O21" s="4"/>
       <c r="P21" s="17"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="22" spans="2:16">
       <c r="B22" s="2" t="s">
         <v>235</v>
       </c>
@@ -2192,7 +2355,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="17"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="23" spans="2:16">
       <c r="B23" s="2" t="s">
         <v>243</v>
       </c>
@@ -2205,14 +2368,24 @@
       <c r="E23" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="G23" s="29"/>
-      <c r="I23" s="29"/>
+      <c r="F23" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>328</v>
+      </c>
       <c r="K23" s="29"/>
       <c r="M23" s="29"/>
       <c r="O23" s="4"/>
       <c r="P23" s="17"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="24" spans="2:16">
       <c r="B24" s="2" t="s">
         <v>247</v>
       </c>
@@ -2252,7 +2425,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="17"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="25" spans="2:16">
       <c r="B25" s="2" t="s">
         <v>259</v>
       </c>
@@ -2292,887 +2465,1076 @@
       <c r="O25" s="4"/>
       <c r="P25" s="17"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.85">
+    <row r="26" spans="2:16">
       <c r="B26" s="2" t="s">
-        <v>271</v>
+        <v>306</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>272</v>
+        <v>319</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="I26" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>288</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="K26" s="29"/>
       <c r="M26" s="29"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.85">
-      <c r="C27" s="29"/>
-      <c r="E27" s="29"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="17"/>
+    </row>
+    <row r="27" spans="2:16">
+      <c r="B27" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>331</v>
+      </c>
       <c r="G27" s="29"/>
       <c r="I27" s="29"/>
       <c r="K27" s="29"/>
       <c r="M27" s="29"/>
-    </row>
-    <row r="28" spans="2:17" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B28" s="30" t="s">
-        <v>299</v>
-      </c>
-      <c r="C28" s="29"/>
-      <c r="E28" s="29"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="17"/>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="B28" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>329</v>
+      </c>
       <c r="G28" s="29"/>
       <c r="I28" s="29"/>
       <c r="K28" s="29"/>
       <c r="M28" s="29"/>
-    </row>
-    <row r="29" spans="2:17" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B29" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" s="25" t="s">
-        <v>1</v>
-      </c>
+      <c r="O28" s="4"/>
+      <c r="P28" s="17"/>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="B29" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="G29" s="29"/>
       <c r="I29" s="29"/>
       <c r="K29" s="29"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="3" t="s">
+      <c r="M29" s="29"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="17"/>
+    </row>
+    <row r="30" spans="2:16">
+      <c r="B30" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="M30" s="29"/>
+    </row>
+    <row r="31" spans="2:16">
+      <c r="C31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="M31" s="29"/>
+    </row>
+    <row r="32" spans="2:16" ht="41" thickBot="1">
+      <c r="B32" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="M32" s="29"/>
+    </row>
+    <row r="33" spans="1:17" ht="41" thickBot="1">
+      <c r="B33" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="N29" s="28"/>
-      <c r="O29" s="3" t="s">
+      <c r="N33" s="28"/>
+      <c r="O33" s="3" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.85">
-      <c r="Q30"/>
-    </row>
-    <row r="31" spans="2:17" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B31" s="18" t="s">
+    <row r="34" spans="1:17">
+      <c r="Q34"/>
+    </row>
+    <row r="35" spans="1:17" ht="41" thickBot="1">
+      <c r="B35" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C35" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D35" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E35" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F35" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="M35" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="N35" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="O35" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q35" s="20" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="B36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="B37" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M37" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="P37" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="41" thickBot="1">
+      <c r="B38" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="L38" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M38" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="P38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q38" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="41" thickBot="1">
+      <c r="B39" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="I39" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M39" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N39" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O39" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q39" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="41" thickBot="1">
+      <c r="B40" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="I40" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M40" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N40" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="O40" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P40" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q40" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="41" thickBot="1">
+      <c r="B41" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M41" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="42" thickTop="1" thickBot="1">
+      <c r="A42" s="17"/>
+      <c r="B42" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="I42" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J42" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L42" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="M42" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="N42" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="O42" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P42" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q42" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="41" thickBot="1">
+      <c r="B43" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L43" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M43" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="41" thickBot="1">
+      <c r="A45" s="20"/>
+      <c r="B45" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G45" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="H31" s="18" t="s">
+      <c r="H45" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="J45" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="I31" s="19" t="s">
+      <c r="K45" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="L45" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="K31" s="20" t="s">
+      <c r="M45" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="L31" s="18" t="s">
+      <c r="N45" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="M31" s="19" t="s">
+      <c r="O45" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="N31" s="4" t="s">
+      <c r="P45" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="O31" s="20" t="s">
+      <c r="Q45" s="20" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.85">
-      <c r="B32" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="N32" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.85">
-      <c r="B33" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="N33" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O33" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B34" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O34" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B35" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L35" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="M35" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O35" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B36" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="M36" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="N36" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O36" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B37" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="M37" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="O37" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="49.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A38" s="17"/>
-      <c r="B38" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F38" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="H38" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I38" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="J38" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="K38" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="L38" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="M38" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="N38" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="O38" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B39" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K39" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="M39" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="O39" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A41" s="20"/>
-      <c r="B41" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="G41" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="I41" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="K41" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="L41" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="M41" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="N41" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="O41" s="20" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.85">
-      <c r="B42" s="2" t="s">
+    <row r="46" spans="1:17">
+      <c r="B46" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H46" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="J46" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="K46" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="L46" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K42" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L42" s="2" t="s">
+      <c r="M46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N46" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="M42" s="3" t="s">
+      <c r="O46" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="N42" s="5" t="s">
+      <c r="P46" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O42" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.85">
-      <c r="B43" s="2" t="s">
+      <c r="Q46" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="B47" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G47" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H47" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="I47" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="K47" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="J43" s="7" t="s">
+      <c r="L47" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K43" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L43" s="2" t="s">
+      <c r="M47" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N47" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="M43" s="3" t="s">
+      <c r="O47" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="N43" s="7" t="s">
+      <c r="P47" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="O43" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B44" s="2" t="s">
+      <c r="Q47" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="41" thickBot="1">
+      <c r="B48" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G48" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H48" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="I48" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="K48" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="J44" s="7" t="s">
+      <c r="L48" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K44" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L44" s="2" t="s">
+      <c r="M48" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N48" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="M44" s="3" t="s">
+      <c r="O48" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="N44" s="7" t="s">
+      <c r="P48" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="O44" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B45" s="2" t="s">
+      <c r="Q48" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="41" thickBot="1">
+      <c r="B49" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F45" s="15" t="s">
+      <c r="E49" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G45" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H45" s="15" t="s">
+      <c r="G49" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="I49" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J49" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I45" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J45" s="4" t="s">
+      <c r="K49" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L49" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K45" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L45" s="15" t="s">
+      <c r="M49" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N49" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="M45" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="N45" s="4" t="s">
+      <c r="O49" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P49" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="O45" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B46" s="2" t="s">
+      <c r="Q49" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="41" thickBot="1">
+      <c r="B50" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F50" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G46" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H46" s="13" t="s">
+      <c r="G50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="I50" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="J50" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I46" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J46" s="4" t="s">
+      <c r="K50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L50" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K46" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L46" s="13" t="s">
+      <c r="M50" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M46" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="N46" s="13" t="s">
+      <c r="O50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P50" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="O46" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B47" s="2" t="s">
+      <c r="Q50" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="41" thickBot="1">
+      <c r="B51" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G51" s="35" t="s">
         <v>212</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H51" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="J51" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="K51" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="J47" s="7" t="s">
+      <c r="L51" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K47" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L47" s="2" t="s">
+      <c r="M51" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N51" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="M47" s="3" t="s">
+      <c r="O51" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="P51" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="O47" s="3" t="s">
+      <c r="Q51" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="49.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A48" s="21"/>
-      <c r="B48" s="11" t="s">
+    <row r="52" spans="1:17" ht="42" thickTop="1" thickBot="1">
+      <c r="A52" s="21"/>
+      <c r="B52" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="24" t="s">
+      <c r="C52" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F48" s="24" t="s">
+      <c r="E52" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G48" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="H48" s="24" t="s">
+      <c r="G52" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H52" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="I52" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J52" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="I48" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="J48" s="26" t="s">
+      <c r="K52" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L52" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="K48" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="L48" s="24" t="s">
+      <c r="M52" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="N52" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="M48" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="N48" s="24" t="s">
+      <c r="O52" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P52" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="O48" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="2:15" ht="48.75" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B49" s="2" t="s">
+      <c r="Q52" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="41" thickBot="1">
+      <c r="B53" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H53" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="I49" s="3" t="s">
+      <c r="K53" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="J49" s="9" t="s">
+      <c r="L53" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K49" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L49" s="2" t="s">
+      <c r="M53" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N53" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="M49" s="3" t="s">
+      <c r="O53" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="N49" s="2" t="s">
+      <c r="P53" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="O49" s="3" t="s">
+      <c r="Q53" s="3" t="s">
         <v>270</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>